<commit_message>
Added Conditional Coupon Bond (including Test and Excel Sheet Modification).
</commit_message>
<xml_diff>
--- a/ShortRateAndIntensity/CorrelatedHullWhiteCIRModelBondPrices.xlsx
+++ b/ShortRateAndIntensity/CorrelatedHullWhiteCIRModelBondPrices.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Desktop\Masterarbeit\Obba\ShortRateAndIntensity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\workspace\MasterthesisAntonSporrer2017\ShortRateAndIntensity\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
   <si>
     <t>Object Viewer</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>Process CIR</t>
+  </si>
+  <si>
+    <t>Conditional Coupon Bond Class</t>
+  </si>
+  <si>
+    <t>Conditional Coupon Bond Price HWModel</t>
   </si>
 </sst>
 </file>
@@ -429,66 +435,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="80"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9.5</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -498,66 +444,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="80"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.0928047472363625E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-2.2618090677689849E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5414555818759675E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.2735618635177904E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.3202091832013581E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.9361759837052479E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.3053457361732617E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-7.7163235703479535E-4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.427487614322369E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-1.8415149183100558E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-1.0821942182110147E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5.4176353024419296E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.5703757797486135E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.1039615160191994E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.1301332350963981E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-5.3616178012824214E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-2.024509166932404E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.9988431168139988E-3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.8342969757039584E-2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -588,10 +474,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>CIRTest!$V$34:$CW$34</c:f>
+              <c:f>CIRTest!$V$57:$AO$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="80"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -657,10 +543,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>CIRTest!$V$35:$CW$35</c:f>
+              <c:f>CIRTest!$V$58:$AO$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="80"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.03</c:v>
                 </c:pt>
@@ -891,6 +777,169 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8D45-4190-BCD4-F70A9E3D4A3A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Coupon Bond</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CIRTest!$V$35:$AO$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CIRTest!$V$37:$AO$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.3132325779667352</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33642400344753925</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3690276244700329</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46112406251985832</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.53366167234891937</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55668154191767749</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60860109930313999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.67786683410789994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79124188986008159</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.93604605954378139</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1409747023277494</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.17882202673366951</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22194965299584354</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.27632503780477136</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.34478459190716848</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.42826656974582861</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.53548923661396142</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.65736100895863425</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.81065426656561768</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0CA7-4E13-8F6F-AD5D9575FCF9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1043,10 +1092,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.81842603674540682"/>
-          <c:y val="0.82624004931985051"/>
-          <c:w val="0.15680906907913106"/>
-          <c:h val="0.15517349986424112"/>
+          <c:x val="0.78311968013344124"/>
+          <c:y val="0.68808735715463876"/>
+          <c:w val="0.1836766665849012"/>
+          <c:h val="0.21686893289847697"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1682,13 +1731,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2211,7 +2260,7 @@
       </c>
       <c r="F10" s="1" t="str">
         <f>[2]!obAddAllJars(F6,F7)</f>
-        <v>C:\Users\Anton\Desktop\Masterarbeit\Obba\ShortRateAndIntensity\lib</v>
+        <v>C:\Users\Anton\workspace\MasterthesisAntonSporrer2017\ShortRateAndIntensity\lib</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2316,7 +2365,7 @@
       </c>
       <c r="F19" s="1" t="str">
         <f>[2]!obAddClasses(F15,F16)</f>
-        <v>C:\Users\Anton\Desktop\Masterarbeit\Obba\ShortRateAndIntensity\Classes</v>
+        <v>C:\Users\Anton\workspace\MasterthesisAntonSporrer2017\ShortRateAndIntensity\Classes</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2379,10 +2428,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CW47"/>
+  <dimension ref="A1:CW58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" topLeftCell="F17" workbookViewId="0">
+      <selection activeCell="V57" sqref="V57:AO58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2401,6 +2450,7 @@
     <col min="21" max="21" width="41.7109375" customWidth="1"/>
     <col min="22" max="22" width="19.140625" customWidth="1"/>
     <col min="23" max="23" width="17.85546875" customWidth="1"/>
+    <col min="41" max="41" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
@@ -2416,114 +2466,6 @@
       <c r="I1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="U1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="U2" t="s">
-        <v>30</v>
-      </c>
-      <c r="V2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",V3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12303]</v>
-      </c>
-      <c r="W2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",W3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12455]</v>
-      </c>
-      <c r="X2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",X3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12542]</v>
-      </c>
-      <c r="Y2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",Y3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12291]</v>
-      </c>
-      <c r="Z2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",Z3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12636]</v>
-      </c>
-      <c r="AA2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AA3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12613]</v>
-      </c>
-      <c r="AB2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AB3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12324]</v>
-      </c>
-      <c r="AC2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AC3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12465]</v>
-      </c>
-      <c r="AD2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AD3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12564]</v>
-      </c>
-      <c r="AE2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AE3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12722]</v>
-      </c>
-      <c r="AF2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AF3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12399]</v>
-      </c>
-      <c r="AG2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AG3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12487]</v>
-      </c>
-      <c r="AH2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AH3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12538]</v>
-      </c>
-      <c r="AI2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AI3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12388]</v>
-      </c>
-      <c r="AJ2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AJ3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12313]</v>
-      </c>
-      <c r="AK2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AK3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12495]</v>
-      </c>
-      <c r="AL2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AL3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12471]</v>
-      </c>
-      <c r="AM2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AM3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12346]</v>
-      </c>
-      <c r="AN2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AN3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12640]</v>
-      </c>
-      <c r="AO2" t="str">
-        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AO3),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12373]</v>
-      </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -2540,75 +2482,12 @@
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="U3" t="s">
-        <v>28</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>1</v>
-      </c>
-      <c r="X3">
-        <v>2</v>
-      </c>
-      <c r="Y3">
-        <v>3</v>
-      </c>
-      <c r="Z3">
-        <v>4</v>
-      </c>
-      <c r="AA3">
-        <v>5</v>
-      </c>
-      <c r="AB3">
-        <v>6</v>
-      </c>
-      <c r="AC3">
-        <v>7</v>
-      </c>
-      <c r="AD3">
-        <v>8</v>
-      </c>
-      <c r="AE3">
-        <v>9</v>
-      </c>
-      <c r="AF3">
-        <v>10</v>
-      </c>
-      <c r="AG3">
-        <v>11</v>
-      </c>
-      <c r="AH3">
-        <v>12</v>
-      </c>
-      <c r="AI3">
-        <v>13</v>
-      </c>
-      <c r="AJ3">
-        <v>14</v>
-      </c>
-      <c r="AK3">
-        <v>15</v>
-      </c>
-      <c r="AL3">
-        <v>16</v>
-      </c>
-      <c r="AM3">
-        <v>17</v>
-      </c>
-      <c r="AN3">
-        <v>18</v>
-      </c>
-      <c r="AO3">
-        <v>19</v>
-      </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>[2]!obMake("td.initialTime", "double",B4)</f>
         <v>td.initialTime 
-[4049]</v>
+[7333]</v>
       </c>
       <c r="B4" s="11">
         <v>0</v>
@@ -2616,110 +2495,27 @@
       <c r="D4" t="str">
         <f>A9</f>
         <v>timeDiscretization2 
-[5484]</v>
+[7788]</v>
       </c>
       <c r="G4" t="str">
         <f>D10</f>
         <v>brownianMotion 
-[12193]</v>
+[7789]</v>
       </c>
       <c r="I4" t="str">
         <f>[2]!obMake("initialValue", "double", J4)</f>
         <v>initialValue 
-[8122]</v>
+[7340]</v>
       </c>
       <c r="J4" s="11">
         <v>0.03</v>
-      </c>
-      <c r="U4" t="s">
-        <v>29</v>
-      </c>
-      <c r="V4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", V3)))</f>
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", W3)))</f>
-        <v>0.5</v>
-      </c>
-      <c r="X4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", X3)))</f>
-        <v>1</v>
-      </c>
-      <c r="Y4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", Y3)))</f>
-        <v>1.5</v>
-      </c>
-      <c r="Z4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", Z3)))</f>
-        <v>2</v>
-      </c>
-      <c r="AA4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AA3)))</f>
-        <v>2.5</v>
-      </c>
-      <c r="AB4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AB3)))</f>
-        <v>3</v>
-      </c>
-      <c r="AC4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AC3)))</f>
-        <v>3.5</v>
-      </c>
-      <c r="AD4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AD3)))</f>
-        <v>4</v>
-      </c>
-      <c r="AE4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AE3)))</f>
-        <v>4.5</v>
-      </c>
-      <c r="AF4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AF3)))</f>
-        <v>5</v>
-      </c>
-      <c r="AG4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AG3)))</f>
-        <v>5.5</v>
-      </c>
-      <c r="AH4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AH3)))</f>
-        <v>6</v>
-      </c>
-      <c r="AI4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AI3)))</f>
-        <v>6.5</v>
-      </c>
-      <c r="AJ4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AJ3)))</f>
-        <v>7</v>
-      </c>
-      <c r="AK4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AK3)))</f>
-        <v>7.5</v>
-      </c>
-      <c r="AL4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AL3)))</f>
-        <v>8</v>
-      </c>
-      <c r="AM4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AM3)))</f>
-        <v>8.5</v>
-      </c>
-      <c r="AN4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AN3)))</f>
-        <v>9</v>
-      </c>
-      <c r="AO4">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AO3)))</f>
-        <v>9.5</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>[2]!obMake("td.numberOfTimeSteps", "int",B5)</f>
         <v>td.numberOfTimeSteps 
-[4620]</v>
+[7332]</v>
       </c>
       <c r="B5" s="11">
         <v>20</v>
@@ -2727,7 +2523,7 @@
       <c r="D5" t="str">
         <f>[2]!obMake("numberOfFactors", "int", E5)</f>
         <v>numberOfFactors 
-[6012]</v>
+[7324]</v>
       </c>
       <c r="E5" s="11">
         <v>1</v>
@@ -2735,97 +2531,17 @@
       <c r="I5" t="str">
         <f>[2]!obMake("kappa","double",J5)</f>
         <v>kappa 
-[8323]</v>
+[7331]</v>
       </c>
       <c r="J5" s="11">
         <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="V5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",V2,"getRealizations") ) )</f>
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",W2,"getRealizations") ) )</f>
-        <v>7.0928047472363625E-3</v>
-      </c>
-      <c r="X5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",X2,"getRealizations") ) )</f>
-        <v>-2.2618090677689849E-2</v>
-      </c>
-      <c r="Y5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",Y2,"getRealizations") ) )</f>
-        <v>1.5414555818759675E-2</v>
-      </c>
-      <c r="Z5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",Z2,"getRealizations") ) )</f>
-        <v>3.2735618635177904E-2</v>
-      </c>
-      <c r="AA5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AA2,"getRealizations") ) )</f>
-        <v>2.3202091832013581E-2</v>
-      </c>
-      <c r="AB5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AB2,"getRealizations") ) )</f>
-        <v>3.9361759837052479E-2</v>
-      </c>
-      <c r="AC5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AC2,"getRealizations") ) )</f>
-        <v>1.3053457361732617E-2</v>
-      </c>
-      <c r="AD5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AD2,"getRealizations") ) )</f>
-        <v>-7.7163235703479535E-4</v>
-      </c>
-      <c r="AE5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AE2,"getRealizations") ) )</f>
-        <v>5.427487614322369E-3</v>
-      </c>
-      <c r="AF5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AF2,"getRealizations") ) )</f>
-        <v>-1.8415149183100558E-2</v>
-      </c>
-      <c r="AG5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AG2,"getRealizations") ) )</f>
-        <v>-1.0821942182110147E-2</v>
-      </c>
-      <c r="AH5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AH2,"getRealizations") ) )</f>
-        <v>5.4176353024419296E-3</v>
-      </c>
-      <c r="AI5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AI2,"getRealizations") ) )</f>
-        <v>3.5703757797486135E-2</v>
-      </c>
-      <c r="AJ5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AJ2,"getRealizations") ) )</f>
-        <v>1.1039615160191994E-2</v>
-      </c>
-      <c r="AK5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AK2,"getRealizations") ) )</f>
-        <v>3.1301332350963981E-2</v>
-      </c>
-      <c r="AL5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AL2,"getRealizations") ) )</f>
-        <v>-5.3616178012824214E-3</v>
-      </c>
-      <c r="AM5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AM2,"getRealizations") ) )</f>
-        <v>-2.024509166932404E-2</v>
-      </c>
-      <c r="AN5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AN2,"getRealizations") ) )</f>
-        <v>4.9988431168139988E-3</v>
-      </c>
-      <c r="AO5">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AO2,"getRealizations") ) )</f>
-        <v>1.8342969757039584E-2</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>[2]!obMake("td.deltaT","double",B6)</f>
         <v>td.deltaT 
-[5150]</v>
+[7787]</v>
       </c>
       <c r="B6" s="11">
         <v>0.5</v>
@@ -2833,7 +2549,7 @@
       <c r="D6" t="str">
         <f>[2]!obMake("numberOfPaths", "int",E6)</f>
         <v>numberOfPaths 
-[9445]</v>
+[7334]</v>
       </c>
       <c r="E6" s="11">
         <v>50</v>
@@ -2844,7 +2560,7 @@
       <c r="I6" t="str">
         <f>[2]!obMake("mu","double",J6)</f>
         <v>mu 
-[1521]</v>
+[7343]</v>
       </c>
       <c r="J6" s="11">
         <v>0.03</v>
@@ -2854,7 +2570,7 @@
       <c r="D7" t="str">
         <f>[2]!obMake("seed","int",E7 )</f>
         <v>seed 
-[12192]</v>
+[7336]</v>
       </c>
       <c r="E7" s="11">
         <v>66</v>
@@ -2862,12 +2578,12 @@
       <c r="G7" t="str">
         <f>[2]!obMake("process", obLibs&amp;"net.finmath.montecarlo.process.ProcessEulerScheme", D10)</f>
         <v>process 
-[12194]</v>
+[7790]</v>
       </c>
       <c r="I7" t="str">
         <f>[2]!obMake("nu","double", J7)</f>
         <v>nu 
-[1513]</v>
+[7341]</v>
       </c>
       <c r="J7" s="11">
         <v>0.03</v>
@@ -2883,7 +2599,7 @@
       <c r="I8" t="str">
         <f>G7</f>
         <v>process 
-[12194]</v>
+[7790]</v>
       </c>
       <c r="U8" t="s">
         <v>37</v>
@@ -2897,7 +2613,7 @@
       <c r="A9" t="str">
         <f>[2]!obMake("timeDiscretization2", obLibs&amp;"net.finmath.time.TimeDiscretization",A4:A6)</f>
         <v>timeDiscretization2 
-[5484]</v>
+[7788]</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>19</v>
@@ -2908,109 +2624,109 @@
       <c r="V9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", V11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12440]</v>
+[8852]</v>
       </c>
       <c r="W9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", W11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12379]</v>
+[8788]</v>
       </c>
       <c r="X9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", X11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12428]</v>
+[8890]</v>
       </c>
       <c r="Y9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", Y11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12600]</v>
+[8831]</v>
       </c>
       <c r="Z9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", Z11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12675]</v>
+[9092]</v>
       </c>
       <c r="AA9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AA11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12299]</v>
+[9031]</v>
       </c>
       <c r="AB9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AB11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12718]</v>
+[8817]</v>
       </c>
       <c r="AC9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AC11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12483]</v>
+[8898]</v>
       </c>
       <c r="AD9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AD11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12681]</v>
+[9063]</v>
       </c>
       <c r="AE9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AE11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12734]</v>
+[9118]</v>
       </c>
       <c r="AF9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AF11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12619]</v>
+[8919]</v>
       </c>
       <c r="AG9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AG11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12582]</v>
+[8988]</v>
       </c>
       <c r="AH9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AH11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12588]</v>
+[8825]</v>
       </c>
       <c r="AI9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AI11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12669]</v>
+[8980]</v>
       </c>
       <c r="AJ9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AJ11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12695]</v>
+[9019]</v>
       </c>
       <c r="AK9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AK11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12309]</v>
+[8968]</v>
       </c>
       <c r="AL9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AL11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12663]</v>
+[9173]</v>
       </c>
       <c r="AM9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AM11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12434]</v>
+[9155]</v>
       </c>
       <c r="AN9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AN11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12338]</v>
+[8868]</v>
       </c>
       <c r="AO9" t="str">
         <f>[2]!obCall("bondPrice", $D$30, "getZeroCouponBond", [2]!obMake("", "double", AO11),[2]!obMake("", "double", $V$8))</f>
         <v>bondPrice 
-[12710]</v>
+[9167]</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="D10" t="str">
         <f>[2]!obMake("brownianMotion", obLibs&amp;"net.finmath.montecarlo.BrownianMotion",D4:D7)</f>
         <v>brownianMotion 
-[12193]</v>
+[7789]</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>19</v>
@@ -3083,7 +2799,7 @@
       <c r="I11" t="str">
         <f>[2]!obMake("cirModel",obLibs&amp;"main.net.finmath.antonsporrer.masterthesis.montecarlo.intensitymodel.CIRModel",I4:I7,G7)</f>
         <v>cirModel 
-[12195]</v>
+[7791]</v>
       </c>
       <c r="U11" t="s">
         <v>36</v>
@@ -3298,7 +3014,7 @@
       <c r="A16" t="str">
         <f>[2]!obMake("interCorrelations", "double[][]",B16:B17)</f>
         <v>interCorrelations 
-[10689]</v>
+[7325]</v>
       </c>
       <c r="B16" s="11">
         <v>0.9</v>
@@ -3307,17 +3023,17 @@
       <c r="D16" t="str">
         <f>A4</f>
         <v>td.initialTime 
-[4049]</v>
+[7333]</v>
       </c>
       <c r="G16" t="str">
         <f>I11</f>
         <v>cirModel 
-[12195]</v>
+[7791]</v>
       </c>
       <c r="I16" t="str">
         <f>[2]!obMake("cva", obLibs&amp;"main.net.finmath.antonsporrer.masterthesis.montecarlo.CVA",D22,G16,A21,D6,D7)</f>
         <v>cva 
-[12196]</v>
+[8233]</v>
       </c>
       <c r="S16" s="10" t="s">
         <v>2</v>
@@ -3325,104 +3041,85 @@
       <c r="U16" t="s">
         <v>30</v>
       </c>
-      <c r="V16" t="str">
+      <c r="V16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", V18), $D$47 )</f>
-        <v>bondPrice 
-[12626]</v>
-      </c>
-      <c r="W16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="W16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", W18), $D$47 )</f>
-        <v>bondPrice 
-[12739]</v>
-      </c>
-      <c r="X16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", X18), $D$47 )</f>
-        <v>bondPrice 
-[12406]</v>
-      </c>
-      <c r="Y16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", Y18), $D$47 )</f>
-        <v>bondPrice 
-[12569]</v>
-      </c>
-      <c r="Z16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", Z18), $D$47 )</f>
-        <v>bondPrice 
-[12351]</v>
-      </c>
-      <c r="AA16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AA18), $D$47 )</f>
-        <v>bondPrice 
-[12500]</v>
-      </c>
-      <c r="AB16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AB18), $D$47 )</f>
-        <v>bondPrice 
-[12417]</v>
-      </c>
-      <c r="AC16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AC16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AC18), $D$47 )</f>
-        <v>bondPrice 
-[12451]</v>
-      </c>
-      <c r="AD16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AD16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AD18), $D$47 )</f>
-        <v>bondPrice 
-[12534]</v>
-      </c>
-      <c r="AE16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AE16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AE18), $D$47 )</f>
-        <v>bondPrice 
-[12395]</v>
-      </c>
-      <c r="AF16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AF16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AF18), $D$47 )</f>
-        <v>bondPrice 
-[12356]</v>
-      </c>
-      <c r="AG16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AG18), $D$47 )</f>
-        <v>bondPrice 
-[12522]</v>
-      </c>
-      <c r="AH16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AH16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AH18), $D$47 )</f>
-        <v>bondPrice 
-[12384]</v>
-      </c>
-      <c r="AI16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AI18), $D$47 )</f>
-        <v>bondPrice 
-[12529]</v>
-      </c>
-      <c r="AJ16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AJ16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AJ18), $D$47 )</f>
-        <v>bondPrice 
-[12704]</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AK16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AK18), $D$47 )</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AL16" t="str">
+      <c r="AL16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AL18), $D$47 )</f>
-        <v>bondPrice 
-[12657]</v>
-      </c>
-      <c r="AM16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AM18), $D$47 )</f>
-        <v>bondPrice 
-[12632]</v>
-      </c>
-      <c r="AN16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AN18), $D$47 )</f>
-        <v>bondPrice 
-[12574]</v>
-      </c>
-      <c r="AO16" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO16" t="e">
         <f>[2]!obCall( "bondPrice", $S$19, "getValue", [2]!obMake("", "double", AO18), $D$47 )</f>
-        <v>bondPrice 
-[12318]</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
@@ -3432,12 +3129,12 @@
       <c r="D17" t="str">
         <f>A5</f>
         <v>td.numberOfTimeSteps 
-[4620]</v>
+[7332]</v>
       </c>
       <c r="S17" t="str">
         <f>[2]!obMake("maturity", "double",V15)</f>
         <v>maturity 
-[1507]</v>
+[7330]</v>
       </c>
       <c r="T17" s="15"/>
       <c r="U17" t="s">
@@ -3508,7 +3205,7 @@
       <c r="D18" t="str">
         <f>A6</f>
         <v>td.deltaT 
-[5150]</v>
+[7787]</v>
       </c>
       <c r="S18" s="10" t="s">
         <v>19</v>
@@ -3602,14 +3299,13 @@
         <v>19</v>
       </c>
       <c r="D19" t="str">
-        <f>[2]!obMake("hullWhiteCreationHelper",  obLibs&amp;"main.net.finmath.antonsporrer.masterthesis.montecarlo.HullWhiteCreationHelper",)</f>
+        <f>[2]!obMake("hullWhiteCreationHelper",  obLibs&amp;"test.net.finmath.antonsporrer.masterthesis.montecarlo.HullWhiteCreationHelper",)</f>
         <v>hullWhiteCreationHelper 
-[1787]</v>
-      </c>
-      <c r="S19" t="str">
+[8231]</v>
+      </c>
+      <c r="S19" t="e">
         <f>[2]!obMake("bond", obLibs&amp;"net.finmath.montecarlo.interestrate.products.Bond", S17)</f>
-        <v>bond 
-[2856]</v>
+        <v>#VALUE!</v>
       </c>
       <c r="U19" t="s">
         <v>45</v>
@@ -3618,81 +3314,81 @@
         <f>[2]!obGet([2]!obCall("", V16, "getRealizations",))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="W19">
+      <c r="W19" t="e">
         <f>[2]!obGet([2]!obCall("", W16, "getRealizations",))</f>
-        <v>3.5880575902361413E-2</v>
-      </c>
-      <c r="X19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X19" t="e">
         <f>[2]!obGet([2]!obCall("", X16, "getRealizations",))</f>
-        <v>3.9155698552943492E-2</v>
-      </c>
-      <c r="Y19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y19" t="e">
         <f>[2]!obGet([2]!obCall("", Y16, "getRealizations",))</f>
-        <v>4.8934303792665536E-2</v>
-      </c>
-      <c r="Z19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z19" t="e">
         <f>[2]!obGet([2]!obCall("", Z16, "getRealizations",))</f>
-        <v>5.6540802862258085E-2</v>
-      </c>
-      <c r="AA19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA19" t="e">
         <f>[2]!obGet([2]!obCall("", AA16, "getRealizations",))</f>
-        <v>5.9893697391905913E-2</v>
-      </c>
-      <c r="AB19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB19" t="e">
         <f>[2]!obGet([2]!obCall("", AB16, "getRealizations",))</f>
-        <v>6.5879322960790854E-2</v>
-      </c>
-      <c r="AC19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AC19" t="e">
         <f>[2]!obGet([2]!obCall("", AC16, "getRealizations",))</f>
-        <v>7.4200894459194741E-2</v>
-      </c>
-      <c r="AD19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AD19" t="e">
         <f>[2]!obGet([2]!obCall("", AD16, "getRealizations",))</f>
-        <v>8.5590869691292287E-2</v>
-      </c>
-      <c r="AE19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AE19" t="e">
         <f>[2]!obGet([2]!obCall("", AE16, "getRealizations",))</f>
-        <v>0.1018554571424711</v>
-      </c>
-      <c r="AF19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AF19" t="e">
         <f>[2]!obGet([2]!obCall("", AF16, "getRealizations",))</f>
-        <v>0.12353350390179368</v>
-      </c>
-      <c r="AG19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG19" t="e">
         <f>[2]!obGet([2]!obCall("", AG16, "getRealizations",))</f>
-        <v>0.15465654438316273</v>
-      </c>
-      <c r="AH19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AH19" t="e">
         <f>[2]!obGet([2]!obCall("", AH16, "getRealizations",))</f>
-        <v>0.19391376876711613</v>
-      </c>
-      <c r="AI19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI19" t="e">
         <f>[2]!obGet([2]!obCall("", AI16, "getRealizations",))</f>
-        <v>0.24612696907811152</v>
-      </c>
-      <c r="AJ19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AJ19" t="e">
         <f>[2]!obGet([2]!obCall("", AJ16, "getRealizations",))</f>
-        <v>0.31446955658421027</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AK19" t="e">
         <f>[2]!obGet([2]!obCall("", AK16, "getRealizations",))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AL19">
+      <c r="AL19" t="e">
         <f>[2]!obGet([2]!obCall("", AL16, "getRealizations",))</f>
-        <v>0.50395363852863784</v>
-      </c>
-      <c r="AM19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM19" t="e">
         <f>[2]!obGet([2]!obCall("", AM16, "getRealizations",))</f>
-        <v>0.63398461761419511</v>
-      </c>
-      <c r="AN19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN19" t="e">
         <f>[2]!obGet([2]!obCall("", AN16, "getRealizations",))</f>
-        <v>0.79405055421236037</v>
-      </c>
-      <c r="AO19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO19" t="e">
         <f>[2]!obGet([2]!obCall("", AO16, "getRealizations",))</f>
-        <v>1</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
@@ -3704,16 +3400,16 @@
         <f>[2]!obGet([2]!obCall("", V16, "getAverage"))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="W20">
+      <c r="W20" t="e">
         <f>[2]!obGet([2]!obCall("", W16, "getAverage"))</f>
-        <v>4.3812030972052378E-2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>[2]!obMake("correlation",  obLibs&amp;"main.net.finmath.antonsporrer.masterthesis.montecarlo.Correlation", A16)</f>
         <v>correlation 
-[10701]</v>
+[8011]</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>19</v>
@@ -3721,9 +3417,9 @@
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="D22" t="str">
-        <f>[2]!obCall("hullWhiteModel",D19,"createHullWhiteModel",D16,D17,D18,U38,U39,U40)</f>
+        <f>[2]!obCall("hullWhiteModel",D19,"createHullWhiteModel",D16,D17,D18,U42,U43,U44)</f>
         <v>hullWhiteModel 
-[5151]</v>
+[8232]</v>
       </c>
       <c r="S22" s="9" t="s">
         <v>44</v>
@@ -3744,104 +3440,104 @@
         <v>35</v>
       </c>
       <c r="V24" t="str">
-        <f>[2]!obCall( "bondPrice"&amp;0, $S$29, "getValue", [2]!obMake("", "double", V26), $D$47 )</f>
+        <f>[2]!obCall( "bondPrice"&amp;0, $S$29, "getValue", [2]!obMake("", "double", V35), $D$47 )</f>
         <v>bondPrice0 
-[12492]</v>
+[9373]</v>
       </c>
       <c r="W24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", W26), $D$47 )</f>
         <v>bondPrice 
-[12747]</v>
+[9410]</v>
       </c>
       <c r="X24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", X26), $D$47 )</f>
         <v>bondPrice 
-[12751]</v>
+[9426]</v>
       </c>
       <c r="Y24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", Y26), $D$47 )</f>
         <v>bondPrice 
-[12755]</v>
+[9422]</v>
       </c>
       <c r="Z24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", Z26), $D$47 )</f>
         <v>bondPrice 
-[12743]</v>
+[9418]</v>
       </c>
       <c r="AA24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AA26), $D$47 )</f>
         <v>bondPrice 
-[12505]</v>
+[9430]</v>
       </c>
       <c r="AB24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AB26), $D$47 )</f>
         <v>bondPrice 
-[12651]</v>
+[9378]</v>
       </c>
       <c r="AC24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AC26), $D$47 )</f>
         <v>bondPrice 
-[12288]</v>
+[9364]</v>
       </c>
       <c r="AD24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AD26), $D$47 )</f>
         <v>bondPrice 
-[12700]</v>
+[9403]</v>
       </c>
       <c r="AE24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AE26), $D$47 )</f>
         <v>bondPrice 
-[12343]</v>
+[9414]</v>
       </c>
       <c r="AF24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AF26), $D$47 )</f>
         <v>bondPrice 
-[12411]</v>
+[9393]</v>
       </c>
       <c r="AG24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AG26), $D$47 )</f>
         <v>bondPrice 
-[12462]</v>
+[9385]</v>
       </c>
       <c r="AH24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AH26), $D$47 )</f>
         <v>bondPrice 
-[12514]</v>
+[9389]</v>
       </c>
       <c r="AI24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AI26), $D$47 )</f>
         <v>bondPrice 
-[12370]</v>
+[9371]</v>
       </c>
       <c r="AJ24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AJ26), $D$47 )</f>
         <v>bondPrice 
-[12509]</v>
+[9391]</v>
       </c>
       <c r="AK24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AK26), $D$47 )</f>
         <v>bondPrice 
-[12363]</v>
+[9366]</v>
       </c>
       <c r="AL24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AL26), $D$47 )</f>
         <v>bondPrice 
-[12607]</v>
+[9382]</v>
       </c>
       <c r="AM24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AM26), $D$47 )</f>
         <v>bondPrice 
-[12547]</v>
+[9407]</v>
       </c>
       <c r="AN24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AN26), $D$47 )</f>
         <v>bondPrice 
-[12422]</v>
+[9395]</v>
       </c>
       <c r="AO24" t="str">
         <f>[2]!obCall( "bondPrice", $S$29, "getValue", [2]!obMake("", "double", AO26), $D$47 )</f>
         <v>bondPrice 
-[12560]</v>
+[9398]</v>
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.25">
@@ -3854,13 +3550,10 @@
       <c r="S25" t="str">
         <f>[2]!obMake("paymentDates", "double[]",Q25:R25 )</f>
         <v>paymentDates 
-[9324]</v>
+[7326]</v>
       </c>
       <c r="U25" t="s">
         <v>28</v>
-      </c>
-      <c r="V25">
-        <v>0</v>
       </c>
       <c r="W25">
         <v>1</v>
@@ -3930,14 +3623,10 @@
       <c r="S26" t="str">
         <f>[2]!obMake("periodFactors", "double[]",Q26:R26 )</f>
         <v>periodFactors 
-[11441]</v>
+[7328]</v>
       </c>
       <c r="U26" t="s">
         <v>36</v>
-      </c>
-      <c r="V26">
-        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",V25)))</f>
-        <v>0</v>
       </c>
       <c r="W26">
         <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",W25)))</f>
@@ -4032,14 +3721,10 @@
       <c r="S27" t="str">
         <f>[2]!obMake("coupons", "double[]",Q27:R27 )</f>
         <v>coupons 
-[11565]</v>
+[7329]</v>
       </c>
       <c r="U27" t="s">
         <v>45</v>
-      </c>
-      <c r="V27">
-        <f>[2]!obGet([2]!obCall("", V24,"getRealizations",  ))</f>
-        <v>3.2664915031436967E-2</v>
       </c>
       <c r="W27">
         <f>[2]!obGet([2]!obCall("", W24,"getRealizations",  ))</f>
@@ -4057,9 +3742,9 @@
         <f>[2]!obGet([2]!obCall("", Z24,"getRealizations",  ))</f>
         <v>5.6540802862258085E-2</v>
       </c>
-      <c r="AA27" t="e">
+      <c r="AA27">
         <f>[2]!obGet([2]!obCall("", AA24,"getRealizations",  ))</f>
-        <v>#VALUE!</v>
+        <v>5.9893697391905913E-2</v>
       </c>
       <c r="AB27" t="e">
         <f>[2]!obGet([2]!obCall("", AB24,"getRealizations",  ))</f>
@@ -4073,9 +3758,9 @@
         <f>[2]!obGet([2]!obCall("", AD24,"getRealizations",  ))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AE27" t="e">
+      <c r="AE27">
         <f>[2]!obGet([2]!obCall("", AE24,"getRealizations",  ))</f>
-        <v>#VALUE!</v>
+        <v>0.1018554571424711</v>
       </c>
       <c r="AF27" t="e">
         <f>[2]!obGet([2]!obCall("", AF24,"getRealizations",  ))</f>
@@ -4089,9 +3774,9 @@
         <f>[2]!obGet([2]!obCall("", AH24,"getRealizations",  ))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AI27" t="e">
+      <c r="AI27">
         <f>[2]!obGet([2]!obCall("", AI24,"getRealizations",  ))</f>
-        <v>#VALUE!</v>
+        <v>0.24612696907811152</v>
       </c>
       <c r="AJ27" t="e">
         <f>[2]!obGet([2]!obCall("", AJ24,"getRealizations",  ))</f>
@@ -4125,10 +3810,6 @@
       <c r="U28" t="s">
         <v>47</v>
       </c>
-      <c r="V28">
-        <f>[2]!obGet([2]!obCall("", V24, "getAverage"))</f>
-        <v>3.9859797337713047E-2</v>
-      </c>
       <c r="W28">
         <f>[2]!obGet([2]!obCall("", W24, "getAverage"))</f>
         <v>4.3812030972052378E-2</v>
@@ -4145,9 +3826,9 @@
         <f>[2]!obGet([2]!obCall("", Z24, "getAverage"))</f>
         <v>6.8666879397555378E-2</v>
       </c>
-      <c r="AA28" t="e">
+      <c r="AA28">
         <f>[2]!obGet([2]!obCall("", AA24, "getAverage"))</f>
-        <v>#VALUE!</v>
+        <v>7.1821426056005458E-2</v>
       </c>
       <c r="AB28" t="e">
         <f>[2]!obGet([2]!obCall("", AB24, "getAverage"))</f>
@@ -4161,9 +3842,9 @@
         <f>[2]!obGet([2]!obCall("", AD24, "getAverage"))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AE28" t="e">
+      <c r="AE28">
         <f>[2]!obGet([2]!obCall("", AE24, "getAverage"))</f>
-        <v>#VALUE!</v>
+        <v>0.11600583570170521</v>
       </c>
       <c r="AF28" t="e">
         <f>[2]!obGet([2]!obCall("", AF24, "getAverage"))</f>
@@ -4181,9 +3862,9 @@
         <f>[2]!obGet([2]!obCall("", AI24, "getAverage"))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AJ28">
+      <c r="AJ28" t="e">
         <f>[2]!obGet([2]!obCall("", AJ24, "getAverage"))</f>
-        <v>0.33725637877195175</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
@@ -4196,361 +3877,307 @@
       <c r="S29" t="str">
         <f>[2]!obMake("couponBond", obLibs&amp;"main.net.finmath.antonsporrer.masterthesis.montecarlo.interestrate.products.CouponBond",S25:S27)</f>
         <v>couponBond 
-[11566]</v>
+[9362]</v>
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="D30" t="str">
         <f>[2]!obCall("correlatedHWModel",  I16, "getUnderlyingModel")</f>
         <v>correlatedHWModel 
-[12198]</v>
+[8777]</v>
       </c>
       <c r="G30" t="str">
         <f>[2]!obCall("correlatedCIRModel", I16, "getIntensityModel")</f>
         <v>correlatedCIRModel 
-[12197]</v>
+[8234]</v>
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="S31" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="U31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="U32" t="s">
-        <v>30</v>
-      </c>
-      <c r="V32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",V33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12260]</v>
-      </c>
-      <c r="W32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",W33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12242]</v>
-      </c>
-      <c r="X32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",X33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12280]</v>
-      </c>
-      <c r="Y32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",Y33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12238]</v>
-      </c>
-      <c r="Z32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",Z33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12210]</v>
-      </c>
-      <c r="AA32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AA33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12218]</v>
-      </c>
-      <c r="AB32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AB33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12202]</v>
-      </c>
-      <c r="AC32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AC33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12268]</v>
-      </c>
-      <c r="AD32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AD33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12222]</v>
-      </c>
-      <c r="AE32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AE33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12254]</v>
-      </c>
-      <c r="AF32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AF33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12250]</v>
-      </c>
-      <c r="AG32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AG33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12272]</v>
-      </c>
-      <c r="AH32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AH33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12246]</v>
-      </c>
-      <c r="AI32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AI33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12206]</v>
-      </c>
-      <c r="AJ32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AJ33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12226]</v>
-      </c>
-      <c r="AK32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AK33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12214]</v>
-      </c>
-      <c r="AL32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AL33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12230]</v>
-      </c>
-      <c r="AM32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AM33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12276]</v>
-      </c>
-      <c r="AN32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AN33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12264]</v>
-      </c>
-      <c r="AO32" t="str">
-        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AO33),[2]!obMake("", "int",0))</f>
-        <v>processValue 
-[12234]</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="4:101" x14ac:dyDescent="0.25">
+      <c r="S33" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="U33" t="s">
+        <v>35</v>
+      </c>
+      <c r="V33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", V35), $D$30)</f>
+        <v>rvCCB 
+[9283]</v>
+      </c>
+      <c r="W33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", W35), $D$30)</f>
+        <v>rvCCB 
+[9287]</v>
+      </c>
+      <c r="X33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", X35), $D$30)</f>
+        <v>rvCCB 
+[9291]</v>
+      </c>
+      <c r="Y33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", Y35), $D$30)</f>
+        <v>rvCCB 
+[9295]</v>
+      </c>
+      <c r="Z33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", Z35), $D$30)</f>
+        <v>rvCCB 
+[9299]</v>
+      </c>
+      <c r="AA33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AA35), $D$30)</f>
+        <v>rvCCB 
+[9303]</v>
+      </c>
+      <c r="AB33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AB35), $D$30)</f>
+        <v>rvCCB 
+[9307]</v>
+      </c>
+      <c r="AC33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AC35), $D$30)</f>
+        <v>rvCCB 
+[9311]</v>
+      </c>
+      <c r="AD33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AD35), $D$30)</f>
+        <v>rvCCB 
+[9315]</v>
+      </c>
+      <c r="AE33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AE35), $D$30)</f>
+        <v>rvCCB 
+[9319]</v>
+      </c>
+      <c r="AF33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AF35), $D$30)</f>
+        <v>rvCCB 
+[9323]</v>
+      </c>
+      <c r="AG33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AG35), $D$30)</f>
+        <v>rvCCB 
+[9327]</v>
+      </c>
+      <c r="AH33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AH35), $D$30)</f>
+        <v>rvCCB 
+[9331]</v>
+      </c>
+      <c r="AI33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AI35), $D$30)</f>
+        <v>rvCCB 
+[9335]</v>
+      </c>
+      <c r="AJ33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AJ35), $D$30)</f>
+        <v>rvCCB 
+[9339]</v>
+      </c>
+      <c r="AK33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AK35), $D$30)</f>
+        <v>rvCCB 
+[9343]</v>
+      </c>
+      <c r="AL33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AL35), $D$30)</f>
+        <v>rvCCB 
+[9347]</v>
+      </c>
+      <c r="AM33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AM35), $D$30)</f>
+        <v>rvCCB 
+[9351]</v>
+      </c>
+      <c r="AN33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AN35), $D$30)</f>
+        <v>rvCCB 
+[9355]</v>
+      </c>
+      <c r="AO33" t="str">
+        <f>[2]!obCall("rvCCB", $S$38, "getValue", [2]!obMake("", "double", AO35), $D$30)</f>
+        <v>rvCCB 
+[9359]</v>
+      </c>
+    </row>
+    <row r="34" spans="4:101" x14ac:dyDescent="0.25">
+      <c r="Q34" s="11">
+        <v>5</v>
+      </c>
+      <c r="R34" s="11">
+        <v>9.5</v>
+      </c>
+      <c r="S34" t="str">
+        <f>[2]!obMake("paymentDatesCCB", "double[]",Q34:R34 )</f>
+        <v>paymentDatesCCB 
+[7327]</v>
+      </c>
+      <c r="U34" t="s">
         <v>28</v>
       </c>
-      <c r="V33">
+      <c r="V34">
         <v>0</v>
       </c>
-      <c r="W33">
+      <c r="W34">
         <v>1</v>
       </c>
-      <c r="X33">
+      <c r="X34">
         <v>2</v>
       </c>
-      <c r="Y33">
+      <c r="Y34">
         <v>3</v>
       </c>
-      <c r="Z33">
+      <c r="Z34">
         <v>4</v>
       </c>
-      <c r="AA33">
+      <c r="AA34">
         <v>5</v>
       </c>
-      <c r="AB33">
+      <c r="AB34">
         <v>6</v>
       </c>
-      <c r="AC33">
+      <c r="AC34">
         <v>7</v>
       </c>
-      <c r="AD33">
+      <c r="AD34">
         <v>8</v>
       </c>
-      <c r="AE33">
+      <c r="AE34">
         <v>9</v>
       </c>
-      <c r="AF33">
+      <c r="AF34">
         <v>10</v>
       </c>
-      <c r="AG33">
+      <c r="AG34">
         <v>11</v>
       </c>
-      <c r="AH33">
+      <c r="AH34">
         <v>12</v>
       </c>
-      <c r="AI33">
+      <c r="AI34">
         <v>13</v>
       </c>
-      <c r="AJ33">
+      <c r="AJ34">
         <v>14</v>
       </c>
-      <c r="AK33">
+      <c r="AK34">
         <v>15</v>
       </c>
-      <c r="AL33">
+      <c r="AL34">
         <v>16</v>
       </c>
-      <c r="AM33">
+      <c r="AM34">
         <v>17</v>
       </c>
-      <c r="AN33">
+      <c r="AN34">
         <v>18</v>
       </c>
-      <c r="AO33">
+      <c r="AO34">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="4:101" x14ac:dyDescent="0.25">
-      <c r="U34" t="s">
-        <v>29</v>
-      </c>
-      <c r="V34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", V33)))</f>
+    <row r="35" spans="4:101" x14ac:dyDescent="0.25">
+      <c r="Q35" s="11">
+        <v>1</v>
+      </c>
+      <c r="R35" s="11">
+        <v>1</v>
+      </c>
+      <c r="S35" t="str">
+        <f>[2]!obMake("periodFactorsCCB", "double[]",Q35:R35 )</f>
+        <v>periodFactorsCCB 
+[7337]</v>
+      </c>
+      <c r="U35" t="s">
+        <v>36</v>
+      </c>
+      <c r="V35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",V34)))</f>
         <v>0</v>
       </c>
-      <c r="W34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", W33)))</f>
+      <c r="W35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",W34)))</f>
         <v>0.5</v>
       </c>
-      <c r="X34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", X33)))</f>
+      <c r="X35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",X34)))</f>
         <v>1</v>
       </c>
-      <c r="Y34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", Y33)))</f>
+      <c r="Y35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",Y34)))</f>
         <v>1.5</v>
       </c>
-      <c r="Z34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", Z33)))</f>
+      <c r="Z35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",Z34)))</f>
         <v>2</v>
       </c>
-      <c r="AA34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AA33)))</f>
+      <c r="AA35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AA34)))</f>
         <v>2.5</v>
       </c>
-      <c r="AB34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AB33)))</f>
+      <c r="AB35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AB34)))</f>
         <v>3</v>
       </c>
-      <c r="AC34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AC33)))</f>
+      <c r="AC35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AC34)))</f>
         <v>3.5</v>
       </c>
-      <c r="AD34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AD33)))</f>
+      <c r="AD35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AD34)))</f>
         <v>4</v>
       </c>
-      <c r="AE34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AE33)))</f>
+      <c r="AE35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AE34)))</f>
         <v>4.5</v>
       </c>
-      <c r="AF34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AF33)))</f>
+      <c r="AF35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AF34)))</f>
         <v>5</v>
       </c>
-      <c r="AG34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AG33)))</f>
+      <c r="AG35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AG34)))</f>
         <v>5.5</v>
       </c>
-      <c r="AH34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AH33)))</f>
+      <c r="AH35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AH34)))</f>
         <v>6</v>
       </c>
-      <c r="AI34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AI33)))</f>
+      <c r="AI35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AI34)))</f>
         <v>6.5</v>
       </c>
-      <c r="AJ34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AJ33)))</f>
+      <c r="AJ35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AJ34)))</f>
         <v>7</v>
       </c>
-      <c r="AK34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AK33)))</f>
+      <c r="AK35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AK34)))</f>
         <v>7.5</v>
       </c>
-      <c r="AL34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AL33)))</f>
+      <c r="AL35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AL34)))</f>
         <v>8</v>
       </c>
-      <c r="AM34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AM33)))</f>
+      <c r="AM35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AM34)))</f>
         <v>8.5</v>
       </c>
-      <c r="AN34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AN33)))</f>
+      <c r="AN35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AN34)))</f>
         <v>9</v>
       </c>
-      <c r="AO34">
-        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AO33)))</f>
+      <c r="AO35">
+        <f>[2]!obGet([2]!obCall("",$D$30,"getTime",[2]!obMake("","int",AO34)))</f>
         <v>9.5</v>
-      </c>
-    </row>
-    <row r="35" spans="4:101" x14ac:dyDescent="0.25">
-      <c r="V35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",V32,"getRealizations") ) )</f>
-        <v>0.03</v>
-      </c>
-      <c r="W35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",W32,"getRealizations") ) )</f>
-        <v>3.1777132373861192E-2</v>
-      </c>
-      <c r="X35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",X32,"getRealizations") ) )</f>
-        <v>2.5172707375884406E-2</v>
-      </c>
-      <c r="Y35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",Y32,"getRealizations") ) )</f>
-        <v>3.1960838339414856E-2</v>
-      </c>
-      <c r="Z35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",Z32,"getRealizations") ) )</f>
-        <v>3.3840837220520031E-2</v>
-      </c>
-      <c r="AA35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AA32,"getRealizations") ) )</f>
-        <v>3.2480960437289846E-2</v>
-      </c>
-      <c r="AB35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AB32,"getRealizations") ) )</f>
-        <v>3.6978724081191697E-2</v>
-      </c>
-      <c r="AC35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AC32,"getRealizations") ) )</f>
-        <v>3.1941410728168793E-2</v>
-      </c>
-      <c r="AD35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AD32,"getRealizations") ) )</f>
-        <v>3.1711474969569164E-2</v>
-      </c>
-      <c r="AE35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AE32,"getRealizations") ) )</f>
-        <v>3.1166386885182605E-2</v>
-      </c>
-      <c r="AF35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AF32,"getRealizations") ) )</f>
-        <v>2.626996237541011E-2</v>
-      </c>
-      <c r="AG35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AG32,"getRealizations") ) )</f>
-        <v>2.9663299105676173E-2</v>
-      </c>
-      <c r="AH35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AH32,"getRealizations") ) )</f>
-        <v>3.429922294563309E-2</v>
-      </c>
-      <c r="AI35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AI32,"getRealizations") ) )</f>
-        <v>4.0869202496482293E-2</v>
-      </c>
-      <c r="AJ35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AJ32,"getRealizations") ) )</f>
-        <v>3.4031785215250056E-2</v>
-      </c>
-      <c r="AK35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AK32,"getRealizations") ) )</f>
-        <v>3.3250779562233178E-2</v>
-      </c>
-      <c r="AL35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AL32,"getRealizations") ) )</f>
-        <v>2.5687678927192415E-2</v>
-      </c>
-      <c r="AM35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AM32,"getRealizations") ) )</f>
-        <v>2.4354483732964154E-2</v>
-      </c>
-      <c r="AN35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AN32,"getRealizations") ) )</f>
-        <v>2.9101683015694671E-2</v>
-      </c>
-      <c r="AO35">
-        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AO32,"getRealizations") ) )</f>
-        <v>3.1743858413575535E-2</v>
       </c>
     </row>
     <row r="36" spans="4:101" x14ac:dyDescent="0.25">
@@ -4559,88 +4186,205 @@
       </c>
       <c r="G36" s="14" t="s">
         <v>48</v>
+      </c>
+      <c r="Q36" s="11">
+        <v>1</v>
+      </c>
+      <c r="R36" s="11">
+        <v>0</v>
+      </c>
+      <c r="S36" t="str">
+        <f>[2]!obMake("couponsCCB", "double[]",Q36:R36 )</f>
+        <v>couponsCCB 
+[7339]</v>
+      </c>
+      <c r="U36" t="s">
+        <v>45</v>
+      </c>
+      <c r="V36">
+        <f>[2]!obGet([2]!obCall("", V33,"getRealizations",  ))</f>
+        <v>0.3132325779667352</v>
+      </c>
+      <c r="W36">
+        <f>[2]!obGet([2]!obCall("", W33,"getRealizations",  ))</f>
+        <v>0.33220734124897311</v>
+      </c>
+      <c r="X36">
+        <f>[2]!obGet([2]!obCall("", X33,"getRealizations",  ))</f>
+        <v>0.41157691414914876</v>
+      </c>
+      <c r="Y36">
+        <f>[2]!obGet([2]!obCall("", Y33,"getRealizations",  ))</f>
+        <v>0.44246724716096186</v>
+      </c>
+      <c r="Z36">
+        <f>[2]!obGet([2]!obCall("", Z33,"getRealizations",  ))</f>
+        <v>0.48352555600816799</v>
+      </c>
+      <c r="AA36">
+        <f>[2]!obGet([2]!obCall("", AA33,"getRealizations",  ))</f>
+        <v>0.52786351233083195</v>
+      </c>
+      <c r="AB36">
+        <f>[2]!obGet([2]!obCall("", AB33,"getRealizations",  ))</f>
+        <v>0.55639168472179912</v>
+      </c>
+      <c r="AC36">
+        <f>[2]!obGet([2]!obCall("", AC33,"getRealizations",  ))</f>
+        <v>0.66463170800246107</v>
+      </c>
+      <c r="AD36">
+        <f>[2]!obGet([2]!obCall("", AD33,"getRealizations",  ))</f>
+        <v>0.78559724497896233</v>
+      </c>
+      <c r="AE36">
+        <f>[2]!obGet([2]!obCall("", AE33,"getRealizations",  ))</f>
+        <v>0.92615938132134601</v>
+      </c>
+      <c r="AF36">
+        <f>[2]!obGet([2]!obCall("", AF33,"getRealizations",  ))</f>
+        <v>1.1472677288713882</v>
+      </c>
+      <c r="AG36">
+        <f>[2]!obGet([2]!obCall("", AG33,"getRealizations",  ))</f>
+        <v>0.17802443387957026</v>
+      </c>
+      <c r="AH36">
+        <f>[2]!obGet([2]!obCall("", AH33,"getRealizations",  ))</f>
+        <v>0.21042605786794541</v>
+      </c>
+      <c r="AI36">
+        <f>[2]!obGet([2]!obCall("", AI33,"getRealizations",  ))</f>
+        <v>0.24227736496642169</v>
+      </c>
+      <c r="AJ36">
+        <f>[2]!obGet([2]!obCall("", AJ33,"getRealizations",  ))</f>
+        <v>0.32563105175533558</v>
+      </c>
+      <c r="AK36">
+        <f>[2]!obGet([2]!obCall("", AK33,"getRealizations",  ))</f>
+        <v>0.39283637829899282</v>
+      </c>
+      <c r="AL36">
+        <f>[2]!obGet([2]!obCall("", AL33,"getRealizations",  ))</f>
+        <v>0.52375225595104236</v>
+      </c>
+      <c r="AM36">
+        <f>[2]!obGet([2]!obCall("", AM33,"getRealizations",  ))</f>
+        <v>0.66004059000004922</v>
+      </c>
+      <c r="AN36">
+        <f>[2]!obGet([2]!obCall("", AN33,"getRealizations",  ))</f>
+        <v>0.80293631088223993</v>
+      </c>
+      <c r="AO36">
+        <f>[2]!obGet([2]!obCall("", AO33,"getRealizations",  ))</f>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="4:101" x14ac:dyDescent="0.25">
       <c r="D37" t="str">
         <f>[2]!obCall("hwProcess",D30, "getProcess")</f>
         <v>hwProcess 
-[12467]</v>
+[8880]</v>
       </c>
       <c r="G37" t="str">
         <f>[2]!obCall("cirProcess",G30, "getProcess")</f>
         <v>cirProcess 
-[12256]</v>
-      </c>
-      <c r="U37" s="9" t="s">
-        <v>34</v>
+[8271]</v>
+      </c>
+      <c r="S37" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="U37" t="s">
+        <v>47</v>
+      </c>
+      <c r="V37">
+        <f>[2]!obGet([2]!obCall("", V33, "getAverage"))</f>
+        <v>0.3132325779667352</v>
+      </c>
+      <c r="W37">
+        <f>[2]!obGet([2]!obCall("", W33, "getAverage"))</f>
+        <v>0.33642400344753925</v>
+      </c>
+      <c r="X37">
+        <f>[2]!obGet([2]!obCall("", X33, "getAverage"))</f>
+        <v>0.3690276244700329</v>
+      </c>
+      <c r="Y37">
+        <f>[2]!obGet([2]!obCall("", Y33, "getAverage"))</f>
+        <v>0.46112406251985832</v>
+      </c>
+      <c r="Z37">
+        <f>[2]!obGet([2]!obCall("", Z33, "getAverage"))</f>
+        <v>0.53366167234891937</v>
+      </c>
+      <c r="AA37">
+        <f>[2]!obGet([2]!obCall("", AA33, "getAverage"))</f>
+        <v>0.55668154191767749</v>
+      </c>
+      <c r="AB37">
+        <f>[2]!obGet([2]!obCall("", AB33, "getAverage"))</f>
+        <v>0.60860109930313999</v>
+      </c>
+      <c r="AC37">
+        <f>[2]!obGet([2]!obCall("", AC33, "getAverage"))</f>
+        <v>0.67786683410789994</v>
+      </c>
+      <c r="AD37">
+        <f>[2]!obGet([2]!obCall("", AD33, "getAverage"))</f>
+        <v>0.79124188986008159</v>
+      </c>
+      <c r="AE37">
+        <f>[2]!obGet([2]!obCall("", AE33, "getAverage"))</f>
+        <v>0.93604605954378139</v>
+      </c>
+      <c r="AF37">
+        <f>[2]!obGet([2]!obCall("", AF33, "getAverage"))</f>
+        <v>1.1409747023277494</v>
+      </c>
+      <c r="AG37">
+        <f>[2]!obGet([2]!obCall("", AG33, "getAverage"))</f>
+        <v>0.17882202673366951</v>
+      </c>
+      <c r="AH37">
+        <f>[2]!obGet([2]!obCall("", AH33, "getAverage"))</f>
+        <v>0.22194965299584354</v>
+      </c>
+      <c r="AI37">
+        <f>[2]!obGet([2]!obCall("", AI33, "getAverage"))</f>
+        <v>0.27632503780477136</v>
+      </c>
+      <c r="AJ37">
+        <f>[2]!obGet([2]!obCall("", AJ33, "getAverage"))</f>
+        <v>0.34478459190716848</v>
+      </c>
+      <c r="AK37">
+        <f>[2]!obGet([2]!obCall("", AK33, "getAverage"))</f>
+        <v>0.42826656974582861</v>
+      </c>
+      <c r="AL37">
+        <f>[2]!obGet([2]!obCall("", AL33, "getAverage"))</f>
+        <v>0.53548923661396142</v>
+      </c>
+      <c r="AM37">
+        <f>[2]!obGet([2]!obCall("", AM33, "getAverage"))</f>
+        <v>0.65736100895863425</v>
+      </c>
+      <c r="AN37">
+        <f>[2]!obGet([2]!obCall("", AN33, "getAverage"))</f>
+        <v>0.81065426656561768</v>
+      </c>
+      <c r="AO37">
+        <f>[2]!obGet([2]!obCall("", AO33, "getAverage"))</f>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="4:101" x14ac:dyDescent="0.25">
-      <c r="U38" t="str">
-        <f>[2]!obMake("meanReversionArrayHW", "double[]",V38:AO38)</f>
-        <v>meanReversionArrayHW 
-[1510]</v>
-      </c>
-      <c r="V38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="W38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="X38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="Y38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="Z38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AA38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AB38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AC38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AD38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AE38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AF38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AG38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AH38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AI38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AJ38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AK38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AL38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AM38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AN38" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="AO38" s="11">
-        <v>0.05</v>
+      <c r="S38" t="str">
+        <f>[2]!obMake("couponBond", obLibs&amp;"main.net.finmath.antonsporrer.masterthesis.montecarlo.interestrate.products.conditionalproducts.ConditionalCouponBond",S34:S36)</f>
+        <v>couponBond 
+[9239]</v>
       </c>
       <c r="AP38" s="12"/>
       <c r="AQ38" s="12"/>
@@ -4710,71 +4454,6 @@
       <c r="G39" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="U39" t="str">
-        <f>[2]!obMake("volatilitesArrayHW", "double[]",V39:AO39)</f>
-        <v>volatilitesArrayHW 
-[1506]</v>
-      </c>
-      <c r="V39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="W39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="X39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="Y39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="Z39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AA39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AB39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AC39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AD39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AE39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AF39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AG39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AH39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AI39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AJ39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AK39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AL39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AM39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AN39" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="AO39" s="11">
-        <v>0.03</v>
-      </c>
       <c r="AP39" s="12"/>
       <c r="AQ39" s="12"/>
       <c r="AR39" s="12"/>
@@ -4840,37 +4519,176 @@
       <c r="D40" t="str">
         <f>[2]!obCall("hwBrownianMotion",D37, "getBrownianMotion")</f>
         <v>hwBrownianMotion 
-[12468]</v>
+[8881]</v>
       </c>
       <c r="G40" t="str">
         <f>[2]!obCall("cirBrownianMotion",G37, "getBrownianMotion")</f>
         <v>cirBrownianMotion 
-[12257]</v>
-      </c>
-      <c r="U40" t="str">
-        <f>[2]!obMake("forwardRateArrayHW", "double[]",V40:Z40)</f>
-        <v>forwardRateArrayHW 
-[1514]</v>
-      </c>
-      <c r="V40" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="W40" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="X40" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="Y40" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="Z40" s="11">
-        <v>0.1</v>
+[8272]</v>
+      </c>
+    </row>
+    <row r="41" spans="4:101" x14ac:dyDescent="0.25">
+      <c r="U41" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="4:101" x14ac:dyDescent="0.25">
+      <c r="U42" t="str">
+        <f>[2]!obMake("meanReversionArrayHW", "double[]",V42:AO42)</f>
+        <v>meanReversionArrayHW 
+[7335]</v>
+      </c>
+      <c r="V42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="W42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="X42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="Y42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="Z42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AA42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AB42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AC42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AD42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AE42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AF42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AG42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AH42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AI42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AJ42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AK42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AL42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AM42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AN42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="AO42" s="11">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="4:101" x14ac:dyDescent="0.25">
+      <c r="U43" t="str">
+        <f>[2]!obMake("volatilitesArrayHW", "double[]",V43:AO43)</f>
+        <v>volatilitesArrayHW 
+[7338]</v>
+      </c>
+      <c r="V43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="W43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="X43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="Y43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="Z43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AA43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AB43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AC43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AD43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AE43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AF43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AG43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AH43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AI43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AJ43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AK43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AL43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AM43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AN43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="AO43" s="11">
+        <v>0.03</v>
       </c>
     </row>
     <row r="44" spans="4:101" x14ac:dyDescent="0.25">
       <c r="D44" s="9" t="s">
         <v>40</v>
+      </c>
+      <c r="U44" t="str">
+        <f>[2]!obMake("forwardRateArrayHW", "double[]",V44:Z44)</f>
+        <v>forwardRateArrayHW 
+[7342]</v>
+      </c>
+      <c r="V44" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="W44" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="X44" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="Y44" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="Z44" s="11">
+        <v>0.1</v>
       </c>
     </row>
     <row r="45" spans="4:101" x14ac:dyDescent="0.25">
@@ -4885,7 +4703,689 @@
       <c r="D47" t="str">
         <f>[2]!obMake("hwTSMMCSimulation", obLibs&amp;"net.finmath.montecarlo.interestrate.TermStructureModelMonteCarloSimulation", D30)</f>
         <v>hwTSMMCSimulation 
-[12199]</v>
+[9126]</v>
+      </c>
+      <c r="U47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="4:101" x14ac:dyDescent="0.25">
+      <c r="U48" t="s">
+        <v>30</v>
+      </c>
+      <c r="V48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",V49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[9069]</v>
+      </c>
+      <c r="W48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",W49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8930]</v>
+      </c>
+      <c r="X48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",X49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[9051]</v>
+      </c>
+      <c r="Y48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",Y49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[9005]</v>
+      </c>
+      <c r="Z48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",Z49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[9023]</v>
+      </c>
+      <c r="AA48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AA49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[9082]</v>
+      </c>
+      <c r="AB48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AB49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8837]</v>
+      </c>
+      <c r="AC48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AC49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[9159]</v>
+      </c>
+      <c r="AD48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AD49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8856]</v>
+      </c>
+      <c r="AE48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AE49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[9129]</v>
+      </c>
+      <c r="AF48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AF49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8811]</v>
+      </c>
+      <c r="AG48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AG49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8934]</v>
+      </c>
+      <c r="AH48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AH49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[9037]</v>
+      </c>
+      <c r="AI48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AI49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8904]</v>
+      </c>
+      <c r="AJ48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AJ49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8950]</v>
+      </c>
+      <c r="AK48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AK49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[9144]</v>
+      </c>
+      <c r="AL48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AL49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8797]</v>
+      </c>
+      <c r="AM48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AM49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8972]</v>
+      </c>
+      <c r="AN48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AN49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[9057]</v>
+      </c>
+      <c r="AO48" t="str">
+        <f>[2]!obCall("processValue",  $D$30, "getProcessValue", [2]!obMake("", "int",AO49),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[9133]</v>
+      </c>
+    </row>
+    <row r="49" spans="21:41" x14ac:dyDescent="0.25">
+      <c r="U49" t="s">
+        <v>28</v>
+      </c>
+      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49">
+        <v>1</v>
+      </c>
+      <c r="X49">
+        <v>2</v>
+      </c>
+      <c r="Y49">
+        <v>3</v>
+      </c>
+      <c r="Z49">
+        <v>4</v>
+      </c>
+      <c r="AA49">
+        <v>5</v>
+      </c>
+      <c r="AB49">
+        <v>6</v>
+      </c>
+      <c r="AC49">
+        <v>7</v>
+      </c>
+      <c r="AD49">
+        <v>8</v>
+      </c>
+      <c r="AE49">
+        <v>9</v>
+      </c>
+      <c r="AF49">
+        <v>10</v>
+      </c>
+      <c r="AG49">
+        <v>11</v>
+      </c>
+      <c r="AH49">
+        <v>12</v>
+      </c>
+      <c r="AI49">
+        <v>13</v>
+      </c>
+      <c r="AJ49">
+        <v>14</v>
+      </c>
+      <c r="AK49">
+        <v>15</v>
+      </c>
+      <c r="AL49">
+        <v>16</v>
+      </c>
+      <c r="AM49">
+        <v>17</v>
+      </c>
+      <c r="AN49">
+        <v>18</v>
+      </c>
+      <c r="AO49">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="21:41" x14ac:dyDescent="0.25">
+      <c r="U50" t="s">
+        <v>29</v>
+      </c>
+      <c r="V50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", V49)))</f>
+        <v>0</v>
+      </c>
+      <c r="W50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", W49)))</f>
+        <v>0.5</v>
+      </c>
+      <c r="X50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", X49)))</f>
+        <v>1</v>
+      </c>
+      <c r="Y50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", Y49)))</f>
+        <v>1.5</v>
+      </c>
+      <c r="Z50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", Z49)))</f>
+        <v>2</v>
+      </c>
+      <c r="AA50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AA49)))</f>
+        <v>2.5</v>
+      </c>
+      <c r="AB50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AB49)))</f>
+        <v>3</v>
+      </c>
+      <c r="AC50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AC49)))</f>
+        <v>3.5</v>
+      </c>
+      <c r="AD50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AD49)))</f>
+        <v>4</v>
+      </c>
+      <c r="AE50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AE49)))</f>
+        <v>4.5</v>
+      </c>
+      <c r="AF50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AF49)))</f>
+        <v>5</v>
+      </c>
+      <c r="AG50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AG49)))</f>
+        <v>5.5</v>
+      </c>
+      <c r="AH50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AH49)))</f>
+        <v>6</v>
+      </c>
+      <c r="AI50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AI49)))</f>
+        <v>6.5</v>
+      </c>
+      <c r="AJ50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AJ49)))</f>
+        <v>7</v>
+      </c>
+      <c r="AK50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AK49)))</f>
+        <v>7.5</v>
+      </c>
+      <c r="AL50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AL49)))</f>
+        <v>8</v>
+      </c>
+      <c r="AM50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AM49)))</f>
+        <v>8.5</v>
+      </c>
+      <c r="AN50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AN49)))</f>
+        <v>9</v>
+      </c>
+      <c r="AO50">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AO49)))</f>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="51" spans="21:41" x14ac:dyDescent="0.25">
+      <c r="V51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",V48,"getRealizations") ) )</f>
+        <v>0</v>
+      </c>
+      <c r="W51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",W48,"getRealizations") ) )</f>
+        <v>7.0928047472363625E-3</v>
+      </c>
+      <c r="X51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",X48,"getRealizations") ) )</f>
+        <v>-2.2618090677689849E-2</v>
+      </c>
+      <c r="Y51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",Y48,"getRealizations") ) )</f>
+        <v>1.5414555818759675E-2</v>
+      </c>
+      <c r="Z51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",Z48,"getRealizations") ) )</f>
+        <v>3.2735618635177904E-2</v>
+      </c>
+      <c r="AA51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AA48,"getRealizations") ) )</f>
+        <v>2.3202091832013581E-2</v>
+      </c>
+      <c r="AB51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AB48,"getRealizations") ) )</f>
+        <v>3.9361759837052479E-2</v>
+      </c>
+      <c r="AC51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AC48,"getRealizations") ) )</f>
+        <v>1.3053457361732617E-2</v>
+      </c>
+      <c r="AD51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AD48,"getRealizations") ) )</f>
+        <v>-7.7163235703479535E-4</v>
+      </c>
+      <c r="AE51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AE48,"getRealizations") ) )</f>
+        <v>5.427487614322369E-3</v>
+      </c>
+      <c r="AF51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AF48,"getRealizations") ) )</f>
+        <v>-1.8415149183100558E-2</v>
+      </c>
+      <c r="AG51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AG48,"getRealizations") ) )</f>
+        <v>-1.0821942182110147E-2</v>
+      </c>
+      <c r="AH51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AH48,"getRealizations") ) )</f>
+        <v>5.4176353024419296E-3</v>
+      </c>
+      <c r="AI51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AI48,"getRealizations") ) )</f>
+        <v>3.5703757797486135E-2</v>
+      </c>
+      <c r="AJ51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AJ48,"getRealizations") ) )</f>
+        <v>1.1039615160191994E-2</v>
+      </c>
+      <c r="AK51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AK48,"getRealizations") ) )</f>
+        <v>3.1301332350963981E-2</v>
+      </c>
+      <c r="AL51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AL48,"getRealizations") ) )</f>
+        <v>-5.3616178012824214E-3</v>
+      </c>
+      <c r="AM51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AM48,"getRealizations") ) )</f>
+        <v>-2.024509166932404E-2</v>
+      </c>
+      <c r="AN51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AN48,"getRealizations") ) )</f>
+        <v>4.9988431168139988E-3</v>
+      </c>
+      <c r="AO51">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AO48,"getRealizations") ) )</f>
+        <v>1.8342969757039584E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="21:41" x14ac:dyDescent="0.25">
+      <c r="U54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="21:41" x14ac:dyDescent="0.25">
+      <c r="U55" t="s">
+        <v>30</v>
+      </c>
+      <c r="V55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",V56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8303]</v>
+      </c>
+      <c r="W55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",W56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8265]</v>
+      </c>
+      <c r="X55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",X56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8315]</v>
+      </c>
+      <c r="Y55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",Y56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8261]</v>
+      </c>
+      <c r="Z55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",Z56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8249]</v>
+      </c>
+      <c r="AA55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AA56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8237]</v>
+      </c>
+      <c r="AB55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AB56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8291]</v>
+      </c>
+      <c r="AC55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AC56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8253]</v>
+      </c>
+      <c r="AD55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AD56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8295]</v>
+      </c>
+      <c r="AE55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AE56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8279]</v>
+      </c>
+      <c r="AF55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AF56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8283]</v>
+      </c>
+      <c r="AG55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AG56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8241]</v>
+      </c>
+      <c r="AH55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AH56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8311]</v>
+      </c>
+      <c r="AI55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AI56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8307]</v>
+      </c>
+      <c r="AJ55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AJ56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8275]</v>
+      </c>
+      <c r="AK55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AK56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8287]</v>
+      </c>
+      <c r="AL55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AL56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8269]</v>
+      </c>
+      <c r="AM55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AM56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8245]</v>
+      </c>
+      <c r="AN55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AN56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8257]</v>
+      </c>
+      <c r="AO55" t="str">
+        <f>[2]!obCall("processValue",  $G$30, "getProcessValue", [2]!obMake("", "int",AO56),[2]!obMake("", "int",0))</f>
+        <v>processValue 
+[8299]</v>
+      </c>
+    </row>
+    <row r="56" spans="21:41" x14ac:dyDescent="0.25">
+      <c r="U56" t="s">
+        <v>28</v>
+      </c>
+      <c r="V56">
+        <v>0</v>
+      </c>
+      <c r="W56">
+        <v>1</v>
+      </c>
+      <c r="X56">
+        <v>2</v>
+      </c>
+      <c r="Y56">
+        <v>3</v>
+      </c>
+      <c r="Z56">
+        <v>4</v>
+      </c>
+      <c r="AA56">
+        <v>5</v>
+      </c>
+      <c r="AB56">
+        <v>6</v>
+      </c>
+      <c r="AC56">
+        <v>7</v>
+      </c>
+      <c r="AD56">
+        <v>8</v>
+      </c>
+      <c r="AE56">
+        <v>9</v>
+      </c>
+      <c r="AF56">
+        <v>10</v>
+      </c>
+      <c r="AG56">
+        <v>11</v>
+      </c>
+      <c r="AH56">
+        <v>12</v>
+      </c>
+      <c r="AI56">
+        <v>13</v>
+      </c>
+      <c r="AJ56">
+        <v>14</v>
+      </c>
+      <c r="AK56">
+        <v>15</v>
+      </c>
+      <c r="AL56">
+        <v>16</v>
+      </c>
+      <c r="AM56">
+        <v>17</v>
+      </c>
+      <c r="AN56">
+        <v>18</v>
+      </c>
+      <c r="AO56">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="21:41" x14ac:dyDescent="0.25">
+      <c r="U57" t="s">
+        <v>29</v>
+      </c>
+      <c r="V57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", V56)))</f>
+        <v>0</v>
+      </c>
+      <c r="W57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", W56)))</f>
+        <v>0.5</v>
+      </c>
+      <c r="X57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", X56)))</f>
+        <v>1</v>
+      </c>
+      <c r="Y57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", Y56)))</f>
+        <v>1.5</v>
+      </c>
+      <c r="Z57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", Z56)))</f>
+        <v>2</v>
+      </c>
+      <c r="AA57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AA56)))</f>
+        <v>2.5</v>
+      </c>
+      <c r="AB57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AB56)))</f>
+        <v>3</v>
+      </c>
+      <c r="AC57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AC56)))</f>
+        <v>3.5</v>
+      </c>
+      <c r="AD57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AD56)))</f>
+        <v>4</v>
+      </c>
+      <c r="AE57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AE56)))</f>
+        <v>4.5</v>
+      </c>
+      <c r="AF57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AF56)))</f>
+        <v>5</v>
+      </c>
+      <c r="AG57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AG56)))</f>
+        <v>5.5</v>
+      </c>
+      <c r="AH57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AH56)))</f>
+        <v>6</v>
+      </c>
+      <c r="AI57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AI56)))</f>
+        <v>6.5</v>
+      </c>
+      <c r="AJ57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AJ56)))</f>
+        <v>7</v>
+      </c>
+      <c r="AK57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AK56)))</f>
+        <v>7.5</v>
+      </c>
+      <c r="AL57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AL56)))</f>
+        <v>8</v>
+      </c>
+      <c r="AM57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AM56)))</f>
+        <v>8.5</v>
+      </c>
+      <c r="AN57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AN56)))</f>
+        <v>9</v>
+      </c>
+      <c r="AO57">
+        <f>[2]!obGet([2]!obCall("",$D$30, "getTime",[2]!obMake("", "int", AO56)))</f>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="58" spans="21:41" x14ac:dyDescent="0.25">
+      <c r="V58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",V55,"getRealizations") ) )</f>
+        <v>0.03</v>
+      </c>
+      <c r="W58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",W55,"getRealizations") ) )</f>
+        <v>3.1777132373861192E-2</v>
+      </c>
+      <c r="X58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",X55,"getRealizations") ) )</f>
+        <v>2.5172707375884406E-2</v>
+      </c>
+      <c r="Y58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",Y55,"getRealizations") ) )</f>
+        <v>3.1960838339414856E-2</v>
+      </c>
+      <c r="Z58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",Z55,"getRealizations") ) )</f>
+        <v>3.3840837220520031E-2</v>
+      </c>
+      <c r="AA58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AA55,"getRealizations") ) )</f>
+        <v>3.2480960437289846E-2</v>
+      </c>
+      <c r="AB58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AB55,"getRealizations") ) )</f>
+        <v>3.6978724081191697E-2</v>
+      </c>
+      <c r="AC58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AC55,"getRealizations") ) )</f>
+        <v>3.1941410728168793E-2</v>
+      </c>
+      <c r="AD58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AD55,"getRealizations") ) )</f>
+        <v>3.1711474969569164E-2</v>
+      </c>
+      <c r="AE58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AE55,"getRealizations") ) )</f>
+        <v>3.1166386885182605E-2</v>
+      </c>
+      <c r="AF58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AF55,"getRealizations") ) )</f>
+        <v>2.626996237541011E-2</v>
+      </c>
+      <c r="AG58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AG55,"getRealizations") ) )</f>
+        <v>2.9663299105676173E-2</v>
+      </c>
+      <c r="AH58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AH55,"getRealizations") ) )</f>
+        <v>3.429922294563309E-2</v>
+      </c>
+      <c r="AI58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AI55,"getRealizations") ) )</f>
+        <v>4.0869202496482293E-2</v>
+      </c>
+      <c r="AJ58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AJ55,"getRealizations") ) )</f>
+        <v>3.4031785215250056E-2</v>
+      </c>
+      <c r="AK58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AK55,"getRealizations") ) )</f>
+        <v>3.3250779562233178E-2</v>
+      </c>
+      <c r="AL58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AL55,"getRealizations") ) )</f>
+        <v>2.5687678927192415E-2</v>
+      </c>
+      <c r="AM58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AM55,"getRealizations") ) )</f>
+        <v>2.4354483732964154E-2</v>
+      </c>
+      <c r="AN58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AN55,"getRealizations") ) )</f>
+        <v>2.9101683015694671E-2</v>
+      </c>
+      <c r="AO58">
+        <f>TRANSPOSE( [2]!obGet([2]!obCall("",AO55,"getRealizations") ) )</f>
+        <v>3.1743858413575535E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>